<commit_message>
when removing scale or trait remove on cascade if no observations related with them
</commit_message>
<xml_diff>
--- a/vavilov3/tests/data/excels/observations_in_columns.xlsx
+++ b/vavilov3/tests/data/excels/observations_in_columns.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Accession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study</t>
+    <t xml:space="preserve">ACCESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUDY</t>
   </si>
   <si>
     <t xml:space="preserve">Plant size:cm</t>
@@ -159,7 +159,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:D4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>